<commit_message>
Update Master Test Plan, Add Group Meeting Minutes Week 6
</commit_message>
<xml_diff>
--- a/Documentation/Risk List/Risk List 1.1.xlsx
+++ b/Documentation/Risk List/Risk List 1.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macuser/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macuser/Library/Mobile Documents/com~apple~CloudDocs/salesAndWarehouseSystem/Documentation/Risk List/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390F7937-85CB-2D4F-AB01-B2B243DDD8D6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6254AE54-6410-834E-A6C8-C4AD8B7E90FC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -574,7 +574,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="122">
   <si>
     <t>ID</t>
   </si>
@@ -590,9 +590,6 @@
   <si>
     <t>Current
 Status</t>
-  </si>
-  <si>
-    <t>&lt;required&gt;</t>
   </si>
   <si>
     <t>Project Name:</t>
@@ -1106,25 +1103,16 @@
     <t>Complete the Project Name, NC, Project Manager Name, and Project Description fields</t>
   </si>
   <si>
-    <t xml:space="preserve">ABC's inventory management system help ABC to get detailed and precise information about the stock movement and stock theft. This also allow employees look up current stock contents of the warehouse and each store and then request stock as required. Employees will also be able to send stock digitally i.e. automatically make an update to the database when stock is sent. Moreover, distribution of stock would also be much easier for the warehouse staff as they will know the quantity of each stock for each store. </t>
-  </si>
-  <si>
     <t>ABC's Inventory Management System</t>
   </si>
   <si>
     <t>Australia</t>
   </si>
   <si>
-    <t>The client does not like the final products.</t>
-  </si>
-  <si>
     <t xml:space="preserve">The team members might be working without any synergy between them, always fighting with each other, blaming and passing the buck, without actual focus on the problem. </t>
   </si>
   <si>
     <t>Closed</t>
-  </si>
-  <si>
-    <t>Group members might not be enough business data to support the project.</t>
   </si>
   <si>
     <t>The project might end up being too complicated. The scopes and functionalities of the project cover too much aspects.</t>
@@ -1151,87 +1139,112 @@
     <t>Reduce or eliminate the unnecessary functionalities base on the non-functional requiremts.</t>
   </si>
   <si>
-    <t>The group does not have much expertise in some of the technology that needs to be used in the project. The system requires to work with XML language but the team members only done some simple task by this language before.</t>
+    <t>Monitor and Prepare</t>
+  </si>
+  <si>
+    <t>Avoidance</t>
+  </si>
+  <si>
+    <t>The team member confirm that he/she could not complete the tasks.</t>
+  </si>
+  <si>
+    <t>The system might not satisfy the client</t>
+  </si>
+  <si>
+    <t>Operation
+Market</t>
+  </si>
+  <si>
+    <t>Conduct the researchs and surveys about the company to get more informaiton about current bussiness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personal issues like work commitment, family, health issues could impact the project or other subject deadlines and exams might affect the schedule of the project. </t>
+  </si>
+  <si>
+    <t>Conduct the meeting between the team and client to get more requirements and feedbacks then re-design or add more functionalities which are required.</t>
+  </si>
+  <si>
+    <t>The project could be delayed or canceled.</t>
+  </si>
+  <si>
+    <t>Making sure that everyone is at a good understanding of the assignment when doing them. Everyone will be expected to stay professional and not prejudge immaturely.</t>
+  </si>
+  <si>
+    <t>Hieu Hanh Tran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Develop an inventory management system which will help ABC to get detailed and precise information about the stock movement, stock information and stock theft. This also allows employees to look up current stock contents of the warehouse and each store and then request stock as required. Employees will also be able to send stock digitally i.e. automatically make an update to the database when stock is sent. Moreover, distribution of stock would also be much easier for the warehouse staff as they will know the quantity of each stock for each store. </t>
+  </si>
+  <si>
+    <t>The group does not have much expertise in some of the technology that needs to be used in the project. The system requires to work with XML and Java EE language but the team members have only done some simple tasks using this language.</t>
   </si>
   <si>
     <t>Schedule
 Performance
-Strategic</t>
-  </si>
-  <si>
-    <t>The team members did not mention XML skills in their resume</t>
-  </si>
-  <si>
-    <t>Discuss about the skill set requirements in the team meeting, if none of the team member could use XML then implement contigency plan</t>
-  </si>
-  <si>
-    <t>Monitor and Prepare</t>
-  </si>
-  <si>
-    <t>Avoidance</t>
-  </si>
-  <si>
-    <t>Change the XML language to other langue which is more farmiliar with the team members.</t>
-  </si>
-  <si>
-    <t>Ask helps from other teams or the expertise in XML.</t>
-  </si>
-  <si>
-    <t>Schedule
-Performance</t>
-  </si>
-  <si>
-    <t>The team members could not attend the team meetings.</t>
-  </si>
-  <si>
-    <t>The team member confirm that he/she could not complete the tasks.</t>
-  </si>
-  <si>
-    <t>Re-schedule the iteration plan to suit with the team members' shcedule</t>
-  </si>
-  <si>
-    <t>The system might not satisfy the client</t>
+Budget</t>
+  </si>
+  <si>
+    <t>The team members not mentioning technical skills in their resume. Team members delaying tasks every week. Team members asking for constant help.</t>
+  </si>
+  <si>
+    <t>Discuss about the skill set requirements in the team meeting, if none of the team member can use XML or Java EE or have basic knowledge about it then implement contigency plan</t>
+  </si>
+  <si>
+    <t>Change the programming languages which is more farmiliar with the team members.</t>
+  </si>
+  <si>
+    <t>Ask help from other teams or the Java EE experts</t>
+  </si>
+  <si>
+    <t>The team members could not attend team meetings.</t>
+  </si>
+  <si>
+    <t>Distribute the affected tasks among other team members untill team member has recovered fully.</t>
+  </si>
+  <si>
+    <t>Re-schedule the iteration plan to suit with the team members' schedule</t>
+  </si>
+  <si>
+    <t>Group members might not have enough business data to support the project.</t>
+  </si>
+  <si>
+    <t>The planning documents such as project proposal, project vision, iteration plan, etc. are confusing and cannot point out the business needs and the project goal.</t>
+  </si>
+  <si>
+    <t>Lack of business data during implementation.</t>
+  </si>
+  <si>
+    <t>Change the dimension of the project</t>
+  </si>
+  <si>
+    <t>The client does not like the final product.</t>
+  </si>
+  <si>
+    <t>The project might restart again or have to be canceled</t>
   </si>
   <si>
     <t>Operation
-Market</t>
-  </si>
-  <si>
-    <t>The planning documents such as project proposal, iteration plan, etc. are confusing and cannot point out the goal of the project.</t>
-  </si>
-  <si>
-    <t>Conduct the researchs and surveys about the company to get more informaiton about current bussiness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Personal issues like work commitment, family, health issues could impact the project or other subject deadlines and exams might affect the schedule of the project. </t>
-  </si>
-  <si>
-    <t>The project might be restart again or have to be put in the canceled</t>
-  </si>
-  <si>
-    <t>Client gave the negative feedbacks through the reports and documents.</t>
-  </si>
-  <si>
-    <t>Conduct the meeting between the team and client to get more requirements and feedbacks then re-design or add more functionalities which are required.</t>
-  </si>
-  <si>
-    <t>The project could be delayed or canceled.</t>
+Market
+Budget
+Schedule</t>
+  </si>
+  <si>
+    <t>Client gives negative feedbacks through reports and documents.</t>
   </si>
   <si>
     <t>Performance
-Operational</t>
-  </si>
-  <si>
-    <t>There are the negative non-verbal actions or fighting in the team meetings.</t>
-  </si>
-  <si>
-    <t>The team members changed/ fixed others'tasks</t>
-  </si>
-  <si>
-    <t>Making sure that everyone is at a good understanding of the assignment when doing them. Everyone will be expected to stay professional and not prejudge immaturely.</t>
-  </si>
-  <si>
-    <t>The manager will have the right to give the punishment to the one did not follow the team rules.</t>
+Operational
+Budget
+Schedule</t>
+  </si>
+  <si>
+    <t>There are negative verbal actions, complains or physical violence in the team meetings.</t>
+  </si>
+  <si>
+    <t>The team members modifying others' tasks</t>
+  </si>
+  <si>
+    <t>The manager will have the right to give punishments to the responsible team members.</t>
   </si>
 </sst>
 </file>
@@ -2128,31 +2141,31 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="12" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2640,168 +2653,168 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14" thickBot="1">
-      <c r="A1" s="93" t="str">
+      <c r="A1" s="100" t="str">
         <f>Risk_Tracking_Log!A1</f>
         <v>RISK MANAGEMENT LOG</v>
       </c>
-      <c r="B1" s="94"/>
+      <c r="B1" s="101"/>
     </row>
     <row r="2" spans="1:2" ht="12" thickBot="1">
       <c r="A2" s="63" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="23"/>
       <c r="B3" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="20"/>
       <c r="B4" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="44">
       <c r="A6" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="66">
       <c r="A7" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="55">
       <c r="A9" s="21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B15" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12" thickBot="1">
       <c r="A17" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B17" s="55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="12" thickBot="1"/>
     <row r="20" spans="1:2" ht="12" thickBot="1">
       <c r="A20" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="34" thickBot="1">
       <c r="A21" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="12" thickBot="1"/>
     <row r="24" spans="1:2" ht="12" thickBot="1">
       <c r="A24" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="56" thickBot="1">
       <c r="A25" s="26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -2820,8 +2833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -2843,7 +2856,7 @@
   <sheetData>
     <row r="1" spans="1:21" s="7" customFormat="1" ht="19" thickBot="1">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -2853,7 +2866,7 @@
       <c r="G1" s="29"/>
       <c r="H1" s="29"/>
       <c r="I1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J1" s="30"/>
       <c r="K1" s="30"/>
@@ -2862,12 +2875,12 @@
     </row>
     <row r="2" spans="1:21" s="1" customFormat="1" ht="14" thickBot="1">
       <c r="A2" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="76"/>
       <c r="C2" s="76"/>
       <c r="D2" s="77" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E2" s="78"/>
       <c r="F2" s="79"/>
@@ -2895,12 +2908,12 @@
     </row>
     <row r="3" spans="1:21" s="1" customFormat="1" ht="14" thickBot="1">
       <c r="A3" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" s="81"/>
       <c r="C3" s="81"/>
       <c r="D3" s="82" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E3" s="83"/>
       <c r="F3" s="84"/>
@@ -2928,12 +2941,12 @@
     </row>
     <row r="4" spans="1:21" s="1" customFormat="1" ht="14" thickBot="1">
       <c r="A4" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="81"/>
       <c r="C4" s="81"/>
       <c r="D4" s="86" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="E4" s="83"/>
       <c r="F4" s="84"/>
@@ -2945,7 +2958,7 @@
       </c>
       <c r="J4" s="86" t="str">
         <f>D4</f>
-        <v>&lt;required&gt;</v>
+        <v>Hieu Hanh Tran</v>
       </c>
       <c r="K4" s="31"/>
       <c r="L4" s="53"/>
@@ -2961,12 +2974,12 @@
     </row>
     <row r="5" spans="1:21" s="1" customFormat="1" ht="128" customHeight="1" thickBot="1">
       <c r="A5" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="76"/>
       <c r="C5" s="87"/>
       <c r="D5" s="64" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="E5" s="88"/>
       <c r="F5" s="88"/>
@@ -2978,7 +2991,7 @@
       </c>
       <c r="J5" s="89" t="str">
         <f>D5</f>
-        <v xml:space="preserve">ABC's inventory management system help ABC to get detailed and precise information about the stock movement and stock theft. This also allow employees look up current stock contents of the warehouse and each store and then request stock as required. Employees will also be able to send stock digitally i.e. automatically make an update to the database when stock is sent. Moreover, distribution of stock would also be much easier for the warehouse staff as they will know the quantity of each stock for each store. </v>
+        <v xml:space="preserve">Develop an inventory management system which will help ABC to get detailed and precise information about the stock movement, stock information and stock theft. This also allows employees to look up current stock contents of the warehouse and each store and then request stock as required. Employees will also be able to send stock digitally i.e. automatically make an update to the database when stock is sent. Moreover, distribution of stock would also be much easier for the warehouse staff as they will know the quantity of each stock for each store. </v>
       </c>
       <c r="K5" s="40"/>
       <c r="L5" s="40"/>
@@ -3000,43 +3013,43 @@
         <v>4</v>
       </c>
       <c r="C6" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="E6" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="42" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" s="44" t="s">
+      <c r="H6" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="44" t="s">
-        <v>57</v>
-      </c>
-      <c r="H6" s="47" t="s">
-        <v>26</v>
-      </c>
       <c r="I6" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="J6" s="42" t="s">
+      <c r="K6" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="L6" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="M6" s="52" t="s">
         <v>51</v>
-      </c>
-      <c r="K6" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="L6" s="44" t="s">
-        <v>75</v>
-      </c>
-      <c r="M6" s="52" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="45" thickBot="1">
       <c r="A7" s="11"/>
       <c r="B7" s="65" t="s">
-        <v>9</v>
+        <v>81</v>
       </c>
       <c r="C7" s="66" t="s">
         <v>2</v>
@@ -3046,37 +3059,37 @@
       </c>
       <c r="E7" s="67" t="str">
         <f>IF(OR(AND(B7&lt;&gt;"Closed",C7="High",D7="High"),AND(B7&lt;&gt;"Closed",C7="High",D7="Medium"),AND(B7&lt;&gt;"Closed",C7="Medium",D7="High")),"Red",IF(OR(AND(B7&lt;&gt;"Closed",C7="High",D7="Low"),AND(B7&lt;&gt;"Closed",C7="Medium",D7="Medium"),AND(B7&lt;&gt;"Closed",C7="Low",D7="High")),"Yellow",IF(OR(AND(B7&lt;&gt;"Closed",C7="Medium",D7="Low"),AND(B7&lt;&gt;"Closed",C7="Low",D7="Low"),AND(B7&lt;&gt;"Closed",C7="Low",D7="Medium")),"Green",IF(B7="Closed","Closed",""))))</f>
-        <v>Yellow</v>
+        <v>Closed</v>
       </c>
       <c r="F7" s="73" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" s="93" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="68" t="s">
+        <v>84</v>
+      </c>
+      <c r="I7" s="94" t="s">
         <v>86</v>
       </c>
-      <c r="G7" s="95" t="s">
+      <c r="J7" s="70" t="s">
         <v>87</v>
       </c>
-      <c r="H7" s="68" t="s">
+      <c r="K7" s="71" t="s">
+        <v>68</v>
+      </c>
+      <c r="L7" s="94" t="s">
+        <v>85</v>
+      </c>
+      <c r="M7" s="95" t="s">
         <v>88</v>
-      </c>
-      <c r="I7" s="96" t="s">
-        <v>90</v>
-      </c>
-      <c r="J7" s="70" t="s">
-        <v>91</v>
-      </c>
-      <c r="K7" s="71" t="s">
-        <v>69</v>
-      </c>
-      <c r="L7" s="96" t="s">
-        <v>89</v>
-      </c>
-      <c r="M7" s="97" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="56" thickBot="1">
       <c r="A8" s="11"/>
       <c r="B8" s="65" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="66" t="s">
         <v>1</v>
@@ -3089,34 +3102,34 @@
         <v>Red</v>
       </c>
       <c r="F8" s="74" t="s">
-        <v>93</v>
-      </c>
-      <c r="G8" s="95" t="s">
-        <v>87</v>
+        <v>101</v>
+      </c>
+      <c r="G8" s="93" t="s">
+        <v>83</v>
       </c>
       <c r="H8" s="68" t="s">
-        <v>94</v>
-      </c>
-      <c r="I8" s="96" t="s">
-        <v>95</v>
-      </c>
-      <c r="J8" s="95" t="s">
-        <v>96</v>
-      </c>
-      <c r="K8" s="98" t="s">
-        <v>98</v>
-      </c>
-      <c r="L8" s="96" t="s">
-        <v>99</v>
-      </c>
-      <c r="M8" s="99" t="s">
-        <v>100</v>
+        <v>102</v>
+      </c>
+      <c r="I8" s="94" t="s">
+        <v>103</v>
+      </c>
+      <c r="J8" s="93" t="s">
+        <v>104</v>
+      </c>
+      <c r="K8" s="96" t="s">
+        <v>90</v>
+      </c>
+      <c r="L8" s="94" t="s">
+        <v>105</v>
+      </c>
+      <c r="M8" s="97" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="34" thickBot="1">
       <c r="A9" s="11"/>
       <c r="B9" s="65" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="66" t="s">
         <v>3</v>
@@ -3129,34 +3142,34 @@
         <v>Yellow</v>
       </c>
       <c r="F9" s="74" t="s">
+        <v>95</v>
+      </c>
+      <c r="G9" s="93" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="68" t="s">
+        <v>102</v>
+      </c>
+      <c r="I9" s="98" t="s">
+        <v>107</v>
+      </c>
+      <c r="J9" s="94" t="s">
+        <v>91</v>
+      </c>
+      <c r="K9" s="99" t="s">
+        <v>89</v>
+      </c>
+      <c r="L9" s="94" t="s">
+        <v>108</v>
+      </c>
+      <c r="M9" s="94" t="s">
         <v>109</v>
       </c>
-      <c r="G9" s="95" t="s">
-        <v>87</v>
-      </c>
-      <c r="H9" s="68" t="s">
-        <v>101</v>
-      </c>
-      <c r="I9" s="100" t="s">
-        <v>102</v>
-      </c>
-      <c r="J9" s="96" t="s">
-        <v>103</v>
-      </c>
-      <c r="K9" s="101" t="s">
-        <v>97</v>
-      </c>
-      <c r="L9" s="96" t="s">
-        <v>99</v>
-      </c>
-      <c r="M9" s="96" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" ht="34" thickBot="1">
+    </row>
+    <row r="10" spans="1:21" ht="45" thickBot="1">
       <c r="A10" s="12"/>
       <c r="B10" s="65" t="s">
-        <v>9</v>
+        <v>81</v>
       </c>
       <c r="C10" s="66" t="s">
         <v>2</v>
@@ -3166,33 +3179,37 @@
       </c>
       <c r="E10" s="67" t="str">
         <f t="shared" si="0"/>
-        <v>Yellow</v>
+        <v>Closed</v>
       </c>
       <c r="F10" s="74" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="G10" s="68" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="H10" s="68" t="s">
-        <v>106</v>
-      </c>
-      <c r="I10" s="100" t="s">
-        <v>107</v>
-      </c>
-      <c r="J10" s="96"/>
+        <v>93</v>
+      </c>
+      <c r="I10" s="98" t="s">
+        <v>111</v>
+      </c>
+      <c r="J10" s="94" t="s">
+        <v>112</v>
+      </c>
       <c r="K10" s="71" t="s">
-        <v>97</v>
-      </c>
-      <c r="L10" s="96" t="s">
-        <v>108</v>
-      </c>
-      <c r="M10" s="96"/>
-    </row>
-    <row r="11" spans="1:21" ht="35" customHeight="1" thickBot="1">
+        <v>89</v>
+      </c>
+      <c r="L10" s="94" t="s">
+        <v>94</v>
+      </c>
+      <c r="M10" s="94" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="46" customHeight="1" thickBot="1">
       <c r="A11" s="12"/>
       <c r="B11" s="65" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="66" t="s">
         <v>2</v>
@@ -3205,30 +3222,30 @@
         <v>Green</v>
       </c>
       <c r="F11" s="74" t="s">
-        <v>82</v>
+        <v>114</v>
       </c>
       <c r="G11" s="68" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="H11" s="68" t="s">
-        <v>106</v>
-      </c>
-      <c r="I11" s="100" t="s">
-        <v>111</v>
-      </c>
-      <c r="J11" s="96"/>
+        <v>116</v>
+      </c>
+      <c r="I11" s="98" t="s">
+        <v>117</v>
+      </c>
+      <c r="J11" s="94"/>
       <c r="K11" s="71" t="s">
-        <v>97</v>
-      </c>
-      <c r="L11" s="96" t="s">
-        <v>112</v>
-      </c>
-      <c r="M11" s="96"/>
+        <v>89</v>
+      </c>
+      <c r="L11" s="94" t="s">
+        <v>96</v>
+      </c>
+      <c r="M11" s="94"/>
     </row>
     <row r="12" spans="1:21" ht="45" thickBot="1">
       <c r="A12" s="12"/>
       <c r="B12" s="65" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C12" s="66" t="s">
         <v>1</v>
@@ -3241,28 +3258,28 @@
         <v>Closed</v>
       </c>
       <c r="F12" s="75" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G12" s="68" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="H12" s="68" t="s">
-        <v>114</v>
-      </c>
-      <c r="I12" s="100" t="s">
-        <v>115</v>
-      </c>
-      <c r="J12" s="96" t="s">
-        <v>116</v>
+        <v>118</v>
+      </c>
+      <c r="I12" s="98" t="s">
+        <v>119</v>
+      </c>
+      <c r="J12" s="94" t="s">
+        <v>120</v>
       </c>
       <c r="K12" s="71" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="L12" s="64" t="s">
-        <v>117</v>
-      </c>
-      <c r="M12" s="96" t="s">
-        <v>118</v>
+        <v>98</v>
+      </c>
+      <c r="M12" s="94" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -3706,102 +3723,102 @@
   <sheetData>
     <row r="1" spans="1:1" ht="14" thickBot="1">
       <c r="A1" s="45" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="46" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="46" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="46" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="46" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="46" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="46" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="46" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="46" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="46" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>